<commit_message>
Remplazo del localhost:3001 por una url publica
</commit_message>
<xml_diff>
--- a/server/excel/registros.xlsx
+++ b/server/excel/registros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Nombre</t>
   </si>
@@ -40,58 +40,79 @@
     <t xml:space="preserve">Ojeda </t>
   </si>
   <si>
-    <t>fútbol</t>
+    <t>baloncesto</t>
   </si>
   <si>
     <t>Masculino</t>
   </si>
   <si>
-    <t>Guatemala</t>
+    <t>Petén</t>
   </si>
   <si>
     <t>Sí</t>
   </si>
   <si>
+    <t>ford, chrysler, toyota, nissan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jose </t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>béisbol</t>
+  </si>
+  <si>
+    <t>No estoy seguro</t>
+  </si>
+  <si>
+    <t>Huehuetenango</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>ford, chrysler</t>
   </si>
   <si>
-    <t>fafda</t>
-  </si>
-  <si>
-    <t>fdagfa</t>
-  </si>
-  <si>
-    <t>natación</t>
-  </si>
-  <si>
-    <t>No estoy seguro</t>
+    <t xml:space="preserve">Maria </t>
+  </si>
+  <si>
+    <t>Gomez</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>ford, toyota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarol </t>
+  </si>
+  <si>
+    <t>Lemus</t>
+  </si>
+  <si>
+    <t>tenis</t>
+  </si>
+  <si>
+    <t>Chiquimula</t>
+  </si>
+  <si>
+    <t>toyota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramos </t>
   </si>
   <si>
     <t>Santa Rosa</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>ford, nissan</t>
-  </si>
-  <si>
-    <t>yayayaya</t>
-  </si>
-  <si>
-    <t>ñañañañaña</t>
-  </si>
-  <si>
-    <t>baloncesto</t>
-  </si>
-  <si>
-    <t>Femenino</t>
-  </si>
-  <si>
-    <t>Chiquimula</t>
-  </si>
-  <si>
-    <t>ford, chrysler, toyota, nissan</t>
+    <t>ford</t>
   </si>
 </sst>
 </file>
@@ -485,13 +506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
@@ -573,19 +594,65 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes para que se guarde en el escritorio
</commit_message>
<xml_diff>
--- a/server/excel/registros.xlsx
+++ b/server/excel/registros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Nombre</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>ford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Villegas </t>
+  </si>
+  <si>
+    <t>natación</t>
+  </si>
+  <si>
+    <t>ford, nissan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruben </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuesta </t>
   </si>
 </sst>
 </file>
@@ -506,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
@@ -655,6 +673,52 @@
         <v>33</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>